<commit_message>
To update List A & B.
</commit_message>
<xml_diff>
--- a/List_A_Relations.xlsx
+++ b/List_A_Relations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8934D71-88CB-4558-BB85-21BD1D01ABED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F1B280-C280-4186-ADB1-2D0526F3D645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
   <si>
     <t>relationshipOfResource</t>
   </si>
@@ -66,6 +66,14 @@
   </si>
   <si>
     <t>姑婆芋</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>密毛魔芋</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>綠背斜紋天蛾</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -444,7 +452,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -527,6 +535,28 @@
         <v>9</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
To add new taxa & object data.
</commit_message>
<xml_diff>
--- a/List_A_Relations.xlsx
+++ b/List_A_Relations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F1B280-C280-4186-ADB1-2D0526F3D645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D4E5572-0606-49C1-BBA7-6CD482326D93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="16">
   <si>
     <t>relationshipOfResource</t>
   </si>
@@ -74,6 +74,14 @@
   </si>
   <si>
     <t>綠背斜紋天蛾</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>五色鳥</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>臺灣海棗</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -452,7 +460,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -504,46 +512,46 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="C7" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -555,6 +563,50 @@
       </c>
       <c r="C9" s="2" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
To update List A.
</commit_message>
<xml_diff>
--- a/List_A_Relations.xlsx
+++ b/List_A_Relations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F53A08-B616-47B4-9E74-FFAF405859F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28832784-DE1E-49D8-A7AB-96EF4ECADCCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -479,7 +479,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>

</xml_diff>